<commit_message>
Added lots of nav and frr questions. Made the tolerances on lollipop distance answers more forgiving
</commit_message>
<xml_diff>
--- a/questions/questions.xlsx
+++ b/questions/questions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="489">
   <si>
     <t>Topic</t>
   </si>
@@ -559,7 +559,7 @@
     <t>Aerobatic flight is prohibited when</t>
   </si>
   <si>
-    <t>below 1500' AGL with &lt;3 sm visibility</t>
+    <t>below 1500' MSL with 4 sm visibility</t>
   </si>
   <si>
     <t>5 nm from centerline of any federal airway</t>
@@ -686,6 +686,798 @@
   </si>
   <si>
     <t>The other aircraft is converging with you going from your left to your right</t>
+  </si>
+  <si>
+    <t>nav</t>
+  </si>
+  <si>
+    <t>What are the four components of dead reckoning?</t>
+  </si>
+  <si>
+    <t>Position, time, speed, and direction</t>
+  </si>
+  <si>
+    <t>Position, time, speed, and distance</t>
+  </si>
+  <si>
+    <t>Position, time, velocity, and direction</t>
+  </si>
+  <si>
+    <t>Altitude, speed, and direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The primary instruments of dead reckoning are </t>
+  </si>
+  <si>
+    <t>Remote Gyro Vertical Compass, Clock, Airspeed Indicator</t>
+  </si>
+  <si>
+    <t>Remote Gyro Vertical Compass, Altimeter, Airspeed Indicator</t>
+  </si>
+  <si>
+    <t>Wet Compass, Clock, Airspeed Indicator</t>
+  </si>
+  <si>
+    <t>Wet Compass, Altimeter, Airspeed Indicator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The secondary instruments of dead reckoning are </t>
+  </si>
+  <si>
+    <t>Altimeter, OAT Gauge</t>
+  </si>
+  <si>
+    <t>Altimeter, OAT Gauge, Wet Compass</t>
+  </si>
+  <si>
+    <t>Altimeter, Wet Compass</t>
+  </si>
+  <si>
+    <t>Wet Compass, OAT Gauge</t>
+  </si>
+  <si>
+    <t>Unless otherwise authorized, which situation always requires a Mode C transponder?</t>
+  </si>
+  <si>
+    <t>Flying in Class E while overflying Class C below 10,000' MSL</t>
+  </si>
+  <si>
+    <t>Landing at an airport with an operating control tower</t>
+  </si>
+  <si>
+    <t>Aircraft within 30 miles of a Class B primary airport below 10,000 feet AGL</t>
+  </si>
+  <si>
+    <t>Flying under the shelf of Class B</t>
+  </si>
+  <si>
+    <t>The difference between compass heading and true heading is</t>
+  </si>
+  <si>
+    <t>Magnetic deviation and magnetic variation</t>
+  </si>
+  <si>
+    <t>magnetic deviation</t>
+  </si>
+  <si>
+    <t>magnetic variation</t>
+  </si>
+  <si>
+    <t>compass variation</t>
+  </si>
+  <si>
+    <t>In order to determine your distance flown, you would multiply time by:</t>
+  </si>
+  <si>
+    <t>Groundspeed</t>
+  </si>
+  <si>
+    <t>Indicated airspeed</t>
+  </si>
+  <si>
+    <t>True airspeed</t>
+  </si>
+  <si>
+    <t>Equivalent airspeed</t>
+  </si>
+  <si>
+    <t>ground</t>
+  </si>
+  <si>
+    <t>The only north seeking instrument in a typical training airplane is:</t>
+  </si>
+  <si>
+    <t>The magnetic compass</t>
+  </si>
+  <si>
+    <t>The heading indicator</t>
+  </si>
+  <si>
+    <t>The BDHI</t>
+  </si>
+  <si>
+    <t>The vertical gyro compass card</t>
+  </si>
+  <si>
+    <t>How many GPS satellites are required to provide a three-dimensional position?</t>
+  </si>
+  <si>
+    <t>If faced with an emergency where Air Traffic Control (ATC) assistance is desired and not already in contact, which frequency can be used to establish communications?</t>
+  </si>
+  <si>
+    <t>121.5 MHz.</t>
+  </si>
+  <si>
+    <t>128.725 MHz.</t>
+  </si>
+  <si>
+    <t>122.5 MHz.</t>
+  </si>
+  <si>
+    <t>137.5 MHz</t>
+  </si>
+  <si>
+    <t>What action is required when two aircraft of the same category converge, but not head-on?</t>
+  </si>
+  <si>
+    <t>The aircraft on the left shall give way.</t>
+  </si>
+  <si>
+    <t>The aircraft on the right shall give way.</t>
+  </si>
+  <si>
+    <t>The faster aircraft shall give way</t>
+  </si>
+  <si>
+    <t>The more maneuverable aircraft shall give way</t>
+  </si>
+  <si>
+    <t>The aircraft that always has right-of-way is the:</t>
+  </si>
+  <si>
+    <t>Aircraft in distress</t>
+  </si>
+  <si>
+    <t>Glider</t>
+  </si>
+  <si>
+    <t>Ballon</t>
+  </si>
+  <si>
+    <t>Aircraft refuelling another aircraft</t>
+  </si>
+  <si>
+    <t>Airport taxiway edge lights are identified at night by</t>
+  </si>
+  <si>
+    <t>blue omnidirectional lights</t>
+  </si>
+  <si>
+    <t>white directional lights.</t>
+  </si>
+  <si>
+    <t>alternate red and green lights</t>
+  </si>
+  <si>
+    <t>white omnidirectional lights</t>
+  </si>
+  <si>
+    <t>An alternating red and green light signal directed from the control tower to an aircraft in flight is a signal to</t>
+  </si>
+  <si>
+    <t>exercise extreme caution</t>
+  </si>
+  <si>
+    <t>not land; the airport is unsafe</t>
+  </si>
+  <si>
+    <t>hold position</t>
+  </si>
+  <si>
+    <t>exit the airspace</t>
+  </si>
+  <si>
+    <t>What does a runway exit sign denote?</t>
+  </si>
+  <si>
+    <t>Direction to a taxiway</t>
+  </si>
+  <si>
+    <t>Designation and direction of a taxiway that leads to a non-movement area</t>
+  </si>
+  <si>
+    <t>Denotes the entrance to a runway from a taxiway</t>
+  </si>
+  <si>
+    <t>Prefered runway exit point</t>
+  </si>
+  <si>
+    <t>An airport's rotating beacon operated during daylight hours indicates</t>
+  </si>
+  <si>
+    <t>that weather at the airport located in Class D airspace is below basic VFR weather minimums.</t>
+  </si>
+  <si>
+    <t>the Air Traffic Control tower is not in operation.</t>
+  </si>
+  <si>
+    <t>there are obstructions on the airport.</t>
+  </si>
+  <si>
+    <t>The airport beacon only operates between sunrise and sunset and never during daylight hours.</t>
+  </si>
+  <si>
+    <t>While on final approach for landing, an alternating green and red light followed by a flashing red light is received from the control tower. Under these circumstances, the pilot should</t>
+  </si>
+  <si>
+    <t>exercise extreme caution and abandon the approach, realizing the airport is unsafe for landing.</t>
+  </si>
+  <si>
+    <t>discontinue the approach, fly the same traffic pattern and approach again, and land.</t>
+  </si>
+  <si>
+    <t>abandon the approach, circle the airport to the right, and expect a flashing white light when the airport is safe for landing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute a low approach with wave off </t>
+  </si>
+  <si>
+    <t>If the control tower uses a light signal to direct a pilot to give way to other aircraft and continue circling, the light will be</t>
+  </si>
+  <si>
+    <t>steady red</t>
+  </si>
+  <si>
+    <t>flashing red</t>
+  </si>
+  <si>
+    <t>flashing white</t>
+  </si>
+  <si>
+    <t>The numbers 35 and 17 on a runway indicate that the runway is oriented approximately:</t>
+  </si>
+  <si>
+    <t>350°; and 170°; magnetic heading.</t>
+  </si>
+  <si>
+    <t>035°; and 017°; magnetic heading.</t>
+  </si>
+  <si>
+    <t>350°; and 170°; true heading.</t>
+  </si>
+  <si>
+    <t>035°; and 017°; true heading.</t>
+  </si>
+  <si>
+    <t>FAA advisory circulars containing subject matter specifically related to general operating and flight rules are issued under which subject number?</t>
+  </si>
+  <si>
+    <t>When two or more aircraft are approaching an airport for the purpose of landing, the right-of-way belongs to the aircraft</t>
+  </si>
+  <si>
+    <t>at the lower altitude</t>
+  </si>
+  <si>
+    <t>that is the least maneuverable</t>
+  </si>
+  <si>
+    <t>that has the other to its right</t>
+  </si>
+  <si>
+    <t>that is going faster</t>
+  </si>
+  <si>
+    <t>The prime meridian, international date line, and equator are all examples of</t>
+  </si>
+  <si>
+    <t>Great Circles</t>
+  </si>
+  <si>
+    <t>Lines of longitude</t>
+  </si>
+  <si>
+    <t>Lines of latitude</t>
+  </si>
+  <si>
+    <t>None of the above</t>
+  </si>
+  <si>
+    <t>All of these are true about lines of longitude EXCEPT</t>
+  </si>
+  <si>
+    <t>The Equator separates the northern and southern hemispheres</t>
+  </si>
+  <si>
+    <t>The prime meridian and international date line are on the same great circle</t>
+  </si>
+  <si>
+    <t>They are all great circles</t>
+  </si>
+  <si>
+    <t>They all intersect at the poles</t>
+  </si>
+  <si>
+    <t>They are used to measure east or west angular distance from the prime meridian</t>
+  </si>
+  <si>
+    <t>The equator is the only great circle line of latitude</t>
+  </si>
+  <si>
+    <t>They are all parallel to each other</t>
+  </si>
+  <si>
+    <t>They are all circular</t>
+  </si>
+  <si>
+    <t>The primary instrument for getting your heading is the</t>
+  </si>
+  <si>
+    <t>Remote gyro vertical compass</t>
+  </si>
+  <si>
+    <t>Wet compass</t>
+  </si>
+  <si>
+    <t>Magnetic compass</t>
+  </si>
+  <si>
+    <t>Attitude indicator</t>
+  </si>
+  <si>
+    <t>Magnetic course is</t>
+  </si>
+  <si>
+    <t>True course correct for magnetic variation</t>
+  </si>
+  <si>
+    <t>True course correct for magnetic deviation</t>
+  </si>
+  <si>
+    <t>True heading correct for magnetic variation</t>
+  </si>
+  <si>
+    <t>True heading correct for magnetic deviation</t>
+  </si>
+  <si>
+    <t>Unless otherwise specified, Federal Airways include that Class E airspace extending upward from</t>
+  </si>
+  <si>
+    <t>1,200' AGL up to and including 17,999' MSL</t>
+  </si>
+  <si>
+    <t>The surface up to and including 18,000' MSL</t>
+  </si>
+  <si>
+    <t>700' AGL up to and including 17,999' MSL</t>
+  </si>
+  <si>
+    <t>1,200' AGL up to and including 18,000' MSL</t>
+  </si>
+  <si>
+    <t>What is the lowest altitude permitted for acrobatic flight?</t>
+  </si>
+  <si>
+    <t>1,500' AGL</t>
+  </si>
+  <si>
+    <t>1,000' AGL</t>
+  </si>
+  <si>
+    <t>3,000' AGL</t>
+  </si>
+  <si>
+    <t>500' AGL</t>
+  </si>
+  <si>
+    <t>The vertical limit of Class C airspace is normally _______ and it's outer circle has a ______ wide diameter</t>
+  </si>
+  <si>
+    <t>4,000' AGL, 8nm</t>
+  </si>
+  <si>
+    <t>4,000' AGL, 4nm</t>
+  </si>
+  <si>
+    <t>2,500' AGL, 4nm</t>
+  </si>
+  <si>
+    <t>SFC, 4,000' MSL, 8nm</t>
+  </si>
+  <si>
+    <t>Pilots flying over a national wildlife refuge are requested to fly no lower than</t>
+  </si>
+  <si>
+    <t>1,500' MSL</t>
+  </si>
+  <si>
+    <t>3,000' MSL</t>
+  </si>
+  <si>
+    <t>Except when necessary for takeoff or landing, what is the minimum safe altitude required for a pilot to operate an aircraft over other than a congested area?</t>
+  </si>
+  <si>
+    <t>An altitude of 500 feet AGL, except over open water or a sparsely populated area, which requires 500 feet from any person, vessel, vehicle, or structure.</t>
+  </si>
+  <si>
+    <t>An altitude of 500 feet above the highest obstacle within a horizontal radius of 1,000 feet.</t>
+  </si>
+  <si>
+    <t>An altitude allowing, if a power unit fails, an emergency landing without undue hazard to persons or property on the surface.</t>
+  </si>
+  <si>
+    <t>1,000 feet above the highest obstacle within a horizontal radius of 2,000 feet of the aircraft.</t>
+  </si>
+  <si>
+    <t>An airspace of defined dimensions, extending from 3 nautical miles outward from the coast of the United States, that contains activity that may be hazardous to nonparticipating aircraft is called:</t>
+  </si>
+  <si>
+    <t>A warning area</t>
+  </si>
+  <si>
+    <t>A prohibited area</t>
+  </si>
+  <si>
+    <t>A restricted area</t>
+  </si>
+  <si>
+    <t>An alert area</t>
+  </si>
+  <si>
+    <t>At what altitude shall the altimeter be set to 29.92, when climbing to cruising flight level?</t>
+  </si>
+  <si>
+    <t>18,000' MSL</t>
+  </si>
+  <si>
+    <t>10,000' MSL</t>
+  </si>
+  <si>
+    <t>10,000' AGL</t>
+  </si>
+  <si>
+    <t>18,000' AGL</t>
+  </si>
+  <si>
+    <t>When flying in a VFR corridor designated through Class B airspace, the maximum speed authorized is</t>
+  </si>
+  <si>
+    <t>250 kts</t>
+  </si>
+  <si>
+    <t>200 kts</t>
+  </si>
+  <si>
+    <t>180 kts</t>
+  </si>
+  <si>
+    <t>150 kts</t>
+  </si>
+  <si>
+    <t>Unless otherwise authorized, what is the maximum indicated airspeed at which a person may operate an aircraft in all locations below 10,000 feet MSL?</t>
+  </si>
+  <si>
+    <t>179 kts</t>
+  </si>
+  <si>
+    <t>149kts</t>
+  </si>
+  <si>
+    <t>No person may take off or land an aircraft under basic VFR at an airport that lies within Class D airspace unless the</t>
+  </si>
+  <si>
+    <t>ground visibility at that airport is at least 3 miles.</t>
+  </si>
+  <si>
+    <t>flight visibility at that airport is at least 3 miles.</t>
+  </si>
+  <si>
+    <t>ground visibility at that airport is at least 1 miles.</t>
+  </si>
+  <si>
+    <t>flight visibility at that airport is at least 1 miles.</t>
+  </si>
+  <si>
+    <t>Pilotage refers to navigating _______</t>
+  </si>
+  <si>
+    <t>with use of ground checkpoints</t>
+  </si>
+  <si>
+    <t>by feel and skill</t>
+  </si>
+  <si>
+    <t>entirely with the instruments inside the cockpit</t>
+  </si>
+  <si>
+    <t>without reference to material of stations exterior to the aircraft</t>
+  </si>
+  <si>
+    <t>A VOR is a ______ based station that provides _______</t>
+  </si>
+  <si>
+    <t>ground, only directional information</t>
+  </si>
+  <si>
+    <t>radar, only directional information</t>
+  </si>
+  <si>
+    <t>ground, directional and distance information</t>
+  </si>
+  <si>
+    <t>radar, directional and distance information</t>
+  </si>
+  <si>
+    <t>VOR stations function strictly</t>
+  </si>
+  <si>
+    <t>Within line of sight</t>
+  </si>
+  <si>
+    <t>With sufficient signal strength</t>
+  </si>
+  <si>
+    <t>When within flying within the signal beam</t>
+  </si>
+  <si>
+    <t>Globally</t>
+  </si>
+  <si>
+    <t>The projection used in aviation maps is called the</t>
+  </si>
+  <si>
+    <t>Lambert conformal projection</t>
+  </si>
+  <si>
+    <t>Mercator projection</t>
+  </si>
+  <si>
+    <t>Cylindrical projection</t>
+  </si>
+  <si>
+    <t>True projection</t>
+  </si>
+  <si>
+    <t>Great circle routes represent the _______ paths between two points and are ________</t>
+  </si>
+  <si>
+    <t>shortest distance, straight lines on lambert conformal projections</t>
+  </si>
+  <si>
+    <t>shortest distance, curved lines on lambert conformal projections</t>
+  </si>
+  <si>
+    <t>constant heading, straight lines on lambert conformal projections</t>
+  </si>
+  <si>
+    <t>constant heading, curved lines on lambert conformal projections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An ONC is a </t>
+  </si>
+  <si>
+    <t>Larger area map</t>
+  </si>
+  <si>
+    <t>More detailed map</t>
+  </si>
+  <si>
+    <t>Navigational aid</t>
+  </si>
+  <si>
+    <t>Ground station</t>
+  </si>
+  <si>
+    <t>A TPC is on the ______ scale as a sectional chart</t>
+  </si>
+  <si>
+    <t>Same</t>
+  </si>
+  <si>
+    <t>Smaller</t>
+  </si>
+  <si>
+    <t>Larger</t>
+  </si>
+  <si>
+    <t>Depends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A TAC is a </t>
+  </si>
+  <si>
+    <t>Chart</t>
+  </si>
+  <si>
+    <t>Navigation Station</t>
+  </si>
+  <si>
+    <t>Air Navigation is primarily concerned with _______</t>
+  </si>
+  <si>
+    <t>Magnetic North</t>
+  </si>
+  <si>
+    <t>True North</t>
+  </si>
+  <si>
+    <t>Geomagnetic North</t>
+  </si>
+  <si>
+    <t>Relative North</t>
+  </si>
+  <si>
+    <t>True variables can be changed into magnetic variables by using</t>
+  </si>
+  <si>
+    <t>Constantly changing magnetic variation</t>
+  </si>
+  <si>
+    <t>Constant magnetic variation</t>
+  </si>
+  <si>
+    <t>Constantly changing magnetic deviation</t>
+  </si>
+  <si>
+    <t>Constant magnetic deviation</t>
+  </si>
+  <si>
+    <t>American time zones are ________ zulu time</t>
+  </si>
+  <si>
+    <t>behind</t>
+  </si>
+  <si>
+    <t>ahead of</t>
+  </si>
+  <si>
+    <t>the same as</t>
+  </si>
+  <si>
+    <t>it depends</t>
+  </si>
+  <si>
+    <t>Zone descriptions ________</t>
+  </si>
+  <si>
+    <t>Shows how many hours ahead or behind zulu time the local time is</t>
+  </si>
+  <si>
+    <t>Shows how many hours ahead or behind the local time zulu time is</t>
+  </si>
+  <si>
+    <t>Shows how many hours ahead or behind zulu time the local time should be based on longitude</t>
+  </si>
+  <si>
+    <t>Shows how many hours ahead or behind the local time zulu time should be based on longitude</t>
+  </si>
+  <si>
+    <t>The equator is the most notable example of</t>
+  </si>
+  <si>
+    <t>Parallels</t>
+  </si>
+  <si>
+    <t>Meridians</t>
+  </si>
+  <si>
+    <t>Small circle routes</t>
+  </si>
+  <si>
+    <t>Radials are</t>
+  </si>
+  <si>
+    <t>Given FROM the station and aligned with magnetic north</t>
+  </si>
+  <si>
+    <t>Given FROM the station and aligned with true north</t>
+  </si>
+  <si>
+    <t>Given TO the station and aligned with true north</t>
+  </si>
+  <si>
+    <t>Given TO the station and aligned with magnetic north</t>
+  </si>
+  <si>
+    <t>The altimeter and OAT gauge are secondary DR instruments because</t>
+  </si>
+  <si>
+    <t>They are used to calculate TAS</t>
+  </si>
+  <si>
+    <t>They can correct errors given from the BDHI</t>
+  </si>
+  <si>
+    <t>They are necessary to account for the third dimension of height</t>
+  </si>
+  <si>
+    <t>They are needed to measure performance</t>
+  </si>
+  <si>
+    <t>The tail of the #2 needle indicates</t>
+  </si>
+  <si>
+    <t>The radial the aircraft is currently on</t>
+  </si>
+  <si>
+    <t>The bearing to the station</t>
+  </si>
+  <si>
+    <t>The aircraft's current heading</t>
+  </si>
+  <si>
+    <t>The reciprocal of the aircraft's current heading</t>
+  </si>
+  <si>
+    <t>The air vector is composed of</t>
+  </si>
+  <si>
+    <t>True heading and True Airspeed</t>
+  </si>
+  <si>
+    <t>True course and True Airspeed</t>
+  </si>
+  <si>
+    <t>Track and Groundspeed</t>
+  </si>
+  <si>
+    <t>Magnetic heading and True Airspeed</t>
+  </si>
+  <si>
+    <t>The wind vector is composed of</t>
+  </si>
+  <si>
+    <t>Wind direction and velocity</t>
+  </si>
+  <si>
+    <t>The ground vector can be composed of</t>
+  </si>
+  <si>
+    <t>Crab angle is the difference of</t>
+  </si>
+  <si>
+    <t>TH and TC measured left or right of TC</t>
+  </si>
+  <si>
+    <t>TH and TC measured left or right of TH</t>
+  </si>
+  <si>
+    <t>TH and TRK measured left or right of TRK</t>
+  </si>
+  <si>
+    <t>TH and TRK measured left or right of TH</t>
+  </si>
+  <si>
+    <t>Drift angle is the difference of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The primary purpose of the jet log is </t>
+  </si>
+  <si>
+    <t>fuel planning</t>
+  </si>
+  <si>
+    <t>calculating the necessary MH to account for wind</t>
+  </si>
+  <si>
+    <t>estimate time a flight will take</t>
+  </si>
+  <si>
+    <t>create a plan to aid with pilotage</t>
+  </si>
+  <si>
+    <t>Navigation that creates a new course determined by the location of a fix is called _______</t>
+  </si>
+  <si>
+    <t>Turn Point Navigation</t>
+  </si>
+  <si>
+    <t>Course Control Navigation</t>
+  </si>
+  <si>
+    <t>Jet Log Navigation</t>
+  </si>
+  <si>
+    <t>Dead Reckoning</t>
   </si>
 </sst>
 </file>
@@ -719,7 +1511,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -727,6 +1519,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -996,7 +1791,7 @@
         <v>13</v>
       </c>
       <c r="H2" s="2">
-        <f t="shared" ref="H2:H47" si="1">ROW()</f>
+        <f t="shared" ref="H2:H105" si="1">ROW()</f>
         <v>2</v>
       </c>
     </row>
@@ -2213,6 +3008,1461 @@
       <c r="H47" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B51" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D55" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="E55" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="F55" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="G55" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H55" s="2">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="H56" s="2">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H57" s="2">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="H58" s="2">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="H59" s="2">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B60" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H60" s="2">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B61" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="H61" s="2">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H62" s="2">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B63" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="H63" s="2">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B64" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="H64" s="2">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B65" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H65" s="2">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B66" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D66" s="1">
+        <v>90.0</v>
+      </c>
+      <c r="E66" s="1">
+        <v>60.0</v>
+      </c>
+      <c r="F66" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="G66" s="1">
+        <v>3710.0</v>
+      </c>
+      <c r="H66" s="2">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B67" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="H67" s="2">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="H68" s="2">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="H69" s="2">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="H70" s="2">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="H71" s="2">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="H72" s="2">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B73" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="H73" s="2">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B74" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="H74" s="2">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B75" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="H75" s="2">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B76" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="H76" s="2">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B77" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="H77" s="2">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B78" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="H78" s="2">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B79" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="H79" s="2">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B80" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="H80" s="2">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B81" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="H81" s="2">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B82" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="H82" s="2">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="H83" s="2">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="H84" s="2">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="H85" s="2">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="H86" s="2">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="H87" s="2">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="H88" s="2">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="H89" s="2">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="H90" s="2">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="H91" s="2">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="H92" s="2">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="H93" s="2">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="H94" s="2">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="H95" s="2">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="H96" s="2">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="H97" s="2">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="H98" s="2">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="H99" s="2">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="H100" s="2">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="H101" s="2">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="H102" s="2">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="E103" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="H103" s="2">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="H104" s="2">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="H105" s="2">
+        <f t="shared" si="1"/>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Editted a few questions
</commit_message>
<xml_diff>
--- a/questions/questions.xlsx
+++ b/questions/questions.xlsx
@@ -757,13 +757,13 @@
     <t>Magnetic deviation and magnetic variation</t>
   </si>
   <si>
-    <t>magnetic deviation</t>
-  </si>
-  <si>
-    <t>magnetic variation</t>
-  </si>
-  <si>
-    <t>compass variation</t>
+    <t>Magnetic deviation</t>
+  </si>
+  <si>
+    <t>Magnetic variation</t>
+  </si>
+  <si>
+    <t>Compass variation</t>
   </si>
   <si>
     <t>In order to determine your distance flown, you would multiply time by:</t>
@@ -967,7 +967,7 @@
     <t>that is going faster</t>
   </si>
   <si>
-    <t>The prime meridian, international date line, and equator are all examples of</t>
+    <t>They are used to measure east or west angular distance from the Prime Meridian</t>
   </si>
   <si>
     <t>Great Circles</t>
@@ -988,7 +988,7 @@
     <t>The Equator separates the northern and southern hemispheres</t>
   </si>
   <si>
-    <t>The prime meridian and international date line are on the same great circle</t>
+    <t>The Prime Meridian and International Date Line are on the same great circle</t>
   </si>
   <si>
     <t>They are all great circles</t>
@@ -1216,7 +1216,7 @@
     <t>With sufficient signal strength</t>
   </si>
   <si>
-    <t>When within flying within the signal beam</t>
+    <t>When flying within the signal beam</t>
   </si>
   <si>
     <t>Globally</t>
@@ -1456,13 +1456,13 @@
     <t>fuel planning</t>
   </si>
   <si>
-    <t>calculating the necessary MH to account for wind</t>
-  </si>
-  <si>
-    <t>estimate time a flight will take</t>
-  </si>
-  <si>
-    <t>create a plan to aid with pilotage</t>
+    <t>to calculate the necessary MH to account for wind</t>
+  </si>
+  <si>
+    <t>to estimate time a flight will take</t>
+  </si>
+  <si>
+    <t>to create a plan to aid with pilotage</t>
   </si>
   <si>
     <t>Navigation that creates a new course determined by the location of a fix is called _______</t>

</xml_diff>

<commit_message>
Edited the one weather question, added some engines questions
</commit_message>
<xml_diff>
--- a/questions/questions.xlsx
+++ b/questions/questions.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="550">
   <si>
     <t>Topic</t>
   </si>
@@ -88,12 +88,12 @@
     <t>Leaving Jacksonville Airport (station pressure 999.7 mb) and traveling to Pensacola airport (station pressure 1033.5 mb) your altimeter will say that the aircraft is _____ than it actually is.</t>
   </si>
   <si>
+    <t>Lower</t>
+  </si>
+  <si>
     <t>Higher</t>
   </si>
   <si>
-    <t>Lower</t>
-  </si>
-  <si>
     <t>Not enough information to determine</t>
   </si>
   <si>
@@ -1478,6 +1478,189 @@
   </si>
   <si>
     <t>Dead Reckoning</t>
+  </si>
+  <si>
+    <t>engines</t>
+  </si>
+  <si>
+    <t>The power control system refers to:</t>
+  </si>
+  <si>
+    <t>The hydraulic system that provides pressure only for the flight controls</t>
+  </si>
+  <si>
+    <t>The part of the AC power system that powers essential equipment for flight</t>
+  </si>
+  <si>
+    <t>The system which controls engine power output, specifically the Power Control Lever, FCUs, and pressurizing and dump valves</t>
+  </si>
+  <si>
+    <t>The part of the lubrication which reacts to engine power output changes</t>
+  </si>
+  <si>
+    <t>The Accumulator works in tandem with the _______ to maintain system pressure during shutdown</t>
+  </si>
+  <si>
+    <t>Check Valve</t>
+  </si>
+  <si>
+    <t>Pressure Relief Valve</t>
+  </si>
+  <si>
+    <t>Pressure Regulator Valve</t>
+  </si>
+  <si>
+    <t>Pressurizing Valve</t>
+  </si>
+  <si>
+    <t>Who discovered the inverse relationship between static and dynamic pressure in a closed system?</t>
+  </si>
+  <si>
+    <t>Bernoulli</t>
+  </si>
+  <si>
+    <t>Pascal</t>
+  </si>
+  <si>
+    <t>Otto</t>
+  </si>
+  <si>
+    <t>Brayton</t>
+  </si>
+  <si>
+    <t>As Engine RPM increases, thrust ________. This effect gets _______ pronounced at higher RPM</t>
+  </si>
+  <si>
+    <t>Increases, more</t>
+  </si>
+  <si>
+    <t>Decreases, less</t>
+  </si>
+  <si>
+    <t>Decreases, more</t>
+  </si>
+  <si>
+    <t>Increases, less</t>
+  </si>
+  <si>
+    <t>As altitude increases, thrust ______</t>
+  </si>
+  <si>
+    <t>Decreases slowly then faster as temperature initially decreases then levels off, while pressure constantly decreases</t>
+  </si>
+  <si>
+    <t>Decreases at a constant rate as temperature decreases and pressure decreases at a faster rate</t>
+  </si>
+  <si>
+    <t>Increases as temperature decreases at a faster rate than pressure decreases</t>
+  </si>
+  <si>
+    <t>Increases initially then decreases as temperature initially decreases then levels off, while pressure constantly decreases</t>
+  </si>
+  <si>
+    <t>Because of ram effect, as airspeed increases, density ______ and thrust ______</t>
+  </si>
+  <si>
+    <t>Increases, increases</t>
+  </si>
+  <si>
+    <t>Increases, decreases</t>
+  </si>
+  <si>
+    <t>Decreases, increases</t>
+  </si>
+  <si>
+    <t>Decreases, decreases</t>
+  </si>
+  <si>
+    <t>As supersonic airflow goes throw a convergent passage, total pressure</t>
+  </si>
+  <si>
+    <t>Remains constant</t>
+  </si>
+  <si>
+    <t>Decreases then Increases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">engines </t>
+  </si>
+  <si>
+    <t>Airflow through a variable geometry inlet duct first go through a _______ passage then a _______ passage in order to maximize _________</t>
+  </si>
+  <si>
+    <t>Convergent, divergent, pressure</t>
+  </si>
+  <si>
+    <t>Convergent, divergent, velocity</t>
+  </si>
+  <si>
+    <t>Divergent, convergent, pressure</t>
+  </si>
+  <si>
+    <t>Divergent, convergent, velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In a reciprocating engine </t>
+  </si>
+  <si>
+    <t>Directly to the crankshaft</t>
+  </si>
+  <si>
+    <t>Directly to the camshaft</t>
+  </si>
+  <si>
+    <t>Through the constant speed drive</t>
+  </si>
+  <si>
+    <t>Through the governor</t>
+  </si>
+  <si>
+    <t>In a dual spool axial compressor GTE, what drives the propeller?</t>
+  </si>
+  <si>
+    <t>The low pressure compressor</t>
+  </si>
+  <si>
+    <t>The high pressure turbine</t>
+  </si>
+  <si>
+    <t>The high pressure compressor</t>
+  </si>
+  <si>
+    <t>Exhaust gases</t>
+  </si>
+  <si>
+    <t>A gas turbine engine is powered by the _____ cycle which occurs _____</t>
+  </si>
+  <si>
+    <t>Brayton, simultaneously</t>
+  </si>
+  <si>
+    <t>Brayton, sequentially</t>
+  </si>
+  <si>
+    <t>Otto, simultaneously</t>
+  </si>
+  <si>
+    <t>Otto, sequentially</t>
+  </si>
+  <si>
+    <t>A reciprocating engine is powered by the _____ cycle which occurs _____</t>
+  </si>
+  <si>
+    <t>Torquemeters measure ______ and are found in _______</t>
+  </si>
+  <si>
+    <t>Shaft horsepower, turbo props and turbo fans</t>
+  </si>
+  <si>
+    <t>Torque, turbo props and turbo fans</t>
+  </si>
+  <si>
+    <t>Foot pounds, turbo props and turbo fans</t>
+  </si>
+  <si>
+    <t>Torque, turbo fans</t>
   </si>
 </sst>
 </file>
@@ -1791,7 +1974,7 @@
         <v>13</v>
       </c>
       <c r="H2" s="2">
-        <f t="shared" ref="H2:H105" si="1">ROW()</f>
+        <f t="shared" ref="H2:H118" si="1">ROW()</f>
         <v>2</v>
       </c>
     </row>
@@ -4463,6 +4646,365 @@
       <c r="H105" s="2">
         <f t="shared" si="1"/>
         <v>105</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B106" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="H106" s="2">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B107" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="H107" s="2">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B108" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="H108" s="2">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B109" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="H109" s="2">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B110" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="H110" s="2">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B111" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="H111" s="2">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B112" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="H112" s="2">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B113" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="H113" s="2">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B114" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="H114" s="2">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B115" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="H115" s="2">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B116" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="H116" s="2">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B117" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="E117" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="F117" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="H117" s="2">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B118" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="H118" s="2">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B119" s="1">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>